<commit_message>
adding writing up about results
</commit_message>
<xml_diff>
--- a/results/Desk Texture Translation PET.xlsx
+++ b/results/Desk Texture Translation PET.xlsx
@@ -619,11 +619,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="436629248"/>
-        <c:axId val="436626896"/>
+        <c:axId val="327605616"/>
+        <c:axId val="327607184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="436629248"/>
+        <c:axId val="327605616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +661,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436626896"/>
+        <c:crossAx val="327607184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -669,7 +669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="436626896"/>
+        <c:axId val="327607184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -715,24 +715,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436629248"/>
+        <c:crossAx val="327605616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="tr"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.57047878748762948"/>
-          <c:y val="3.9748953974895397E-2"/>
-          <c:w val="0.18642356180887226"/>
-          <c:h val="0.15412809277501399"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:schemeClr val="lt1"/>
@@ -1267,11 +1258,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="436630424"/>
-        <c:axId val="436624544"/>
+        <c:axId val="327608360"/>
+        <c:axId val="327602872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="436630424"/>
+        <c:axId val="327608360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +1300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436624544"/>
+        <c:crossAx val="327602872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1317,7 +1308,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="436624544"/>
+        <c:axId val="327602872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1363,7 +1354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="436630424"/>
+        <c:crossAx val="327608360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1778,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating writing and updating one of the tables
</commit_message>
<xml_diff>
--- a/results/Desk Texture Translation PET.xlsx
+++ b/results/Desk Texture Translation PET.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Apartment.Texture.rotate</t>
   </si>
@@ -67,6 +67,21 @@
   </si>
   <si>
     <t>PCA</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>min-error</t>
+  </si>
+  <si>
+    <t>pct</t>
+  </si>
+  <si>
+    <t>fm2d</t>
+  </si>
+  <si>
+    <t>fvr</t>
   </si>
 </sst>
 </file>
@@ -619,11 +634,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="327605616"/>
-        <c:axId val="327607184"/>
+        <c:axId val="191657120"/>
+        <c:axId val="191655944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="327605616"/>
+        <c:axId val="191657120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +676,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327607184"/>
+        <c:crossAx val="191655944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -669,7 +684,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327607184"/>
+        <c:axId val="191655944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3"/>
@@ -715,7 +730,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327605616"/>
+        <c:crossAx val="191657120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1258,11 +1273,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="327608360"/>
-        <c:axId val="327602872"/>
+        <c:axId val="191659864"/>
+        <c:axId val="191657904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="327608360"/>
+        <c:axId val="191659864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1315,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327602872"/>
+        <c:crossAx val="191657904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1308,7 +1323,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="327602872"/>
+        <c:axId val="191657904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1354,7 +1369,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="327608360"/>
+        <c:crossAx val="191659864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1418,7 +1433,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="75" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -1456,7 +1471,7 @@
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
-    <xdr:pos x="6372225" y="2247900"/>
+    <xdr:pos x="6343650" y="66675"/>
     <xdr:ext cx="6191249" cy="3746500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1767,10 +1782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2202,7 +2217,7 @@
         <v>80.693700000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2232,7 +2247,7 @@
         <v>9.4628399999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2262,7 +2277,7 @@
         <v>7.1522199999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2292,7 +2307,7 @@
         <v>27.366800000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2322,7 +2337,7 @@
         <v>0.488927</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2352,7 +2367,7 @@
         <v>0.68646200000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2382,7 +2397,7 @@
         <v>1.8574900000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2412,7 +2427,7 @@
         <v>3.55674</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2442,7 +2457,7 @@
         <v>554.46799999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2472,7 +2487,7 @@
         <v>1.99396</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2502,7 +2517,7 @@
         <v>3.5805099999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2532,7 +2547,7 @@
         <v>1.43777</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2562,7 +2577,7 @@
         <v>1.0854600000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -2593,8 +2608,26 @@
       <c r="J30" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" t="s">
+        <v>2</v>
+      </c>
+      <c r="O30" t="s">
+        <v>3</v>
+      </c>
+      <c r="P30" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2634,925 +2667,1545 @@
         <f>MIN(G31:I31)</f>
         <v>1.0750067751551833</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <f>MIN(C31:J31)</f>
+        <v>0.89382751100156155</v>
+      </c>
+      <c r="M31">
+        <f>IF($L31=C31,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ref="N31:Q46" si="2">IF($L31=D31,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <f>IF($L31=J31,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>A31+1</f>
         <v>2</v>
       </c>
       <c r="B32">
-        <f t="shared" ref="B32:B53" si="2">B5</f>
+        <f t="shared" ref="B32:B53" si="3">B5</f>
         <v>0.62565400000000004</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:I32" si="3">C5/$B32</f>
+        <f t="shared" ref="C32:I32" si="4">C5/$B32</f>
         <v>0.79454139188752881</v>
       </c>
       <c r="D32">
+        <f t="shared" si="4"/>
+        <v>0.9863918395790644</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="4"/>
+        <v>0.54356721127012697</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>0.97153378704523585</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="4"/>
+        <v>0.51662260610497168</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>0.57050542312524177</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="4"/>
+        <v>0.58853615576660578</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32:J53" si="5">MIN(G32:I32)</f>
+        <v>0.51662260610497168</v>
+      </c>
+      <c r="L32">
+        <f t="shared" ref="L32:L53" si="6">MIN(C32:J32)</f>
+        <v>0.51662260610497168</v>
+      </c>
+      <c r="M32">
+        <f t="shared" ref="M32:P53" si="7">IF($L32=C32,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ref="Q32:Q53" si="8">IF($L32=J32,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" ref="A33:A53" si="9">A32+1</f>
+        <v>3</v>
+      </c>
+      <c r="B33">
         <f t="shared" si="3"/>
-        <v>0.9863918395790644</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="3"/>
-        <v>0.54356721127012697</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="3"/>
-        <v>0.97153378704523585</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="3"/>
-        <v>0.51662260610497168</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="3"/>
-        <v>0.57050542312524177</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="3"/>
-        <v>0.58853615576660578</v>
-      </c>
-      <c r="J32">
-        <f t="shared" ref="J32:J53" si="4">MIN(G32:I32)</f>
-        <v>0.51662260610497168</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <f t="shared" ref="A33:A53" si="5">A32+1</f>
-        <v>3</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="2"/>
         <v>0.54721299999999995</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:I33" si="6">C6/$B33</f>
+        <f t="shared" ref="C33:I33" si="10">C6/$B33</f>
         <v>0.83401710120190864</v>
       </c>
       <c r="D33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.72505404659611528</v>
       </c>
       <c r="E33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.8871719056382068</v>
       </c>
       <c r="F33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.6971691096520003</v>
       </c>
       <c r="G33">
+        <f t="shared" si="10"/>
+        <v>0.68360949027161277</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="10"/>
+        <v>1.054348124039451</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="10"/>
+        <v>0.81598755877510232</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="5"/>
+        <v>0.68360949027161277</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="6"/>
         <v>0.68360949027161277</v>
       </c>
-      <c r="H33">
+      <c r="M33">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="3"/>
+        <v>0.79624799999999996</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:I34" si="11">C7/$B34</f>
+        <v>1.2344809657292704</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="11"/>
+        <v>5.2802016457184191</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="11"/>
+        <v>1.117418191317278</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="11"/>
+        <v>0.83349031959891895</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="11"/>
+        <v>1.0258801277993792</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="11"/>
+        <v>1.3056233736222886</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="11"/>
+        <v>1.6220197727341232</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="5"/>
+        <v>1.0258801277993792</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="6"/>
-        <v>1.054348124039451</v>
-      </c>
-      <c r="I33">
+        <v>0.83349031959891895</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="3"/>
+        <v>1.3063899999999999</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35:I35" si="12">C8/$B35</f>
+        <v>0.89705218196710013</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="12"/>
+        <v>0.96674040676980078</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="12"/>
+        <v>0.66196005786939593</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="12"/>
+        <v>1.1933266482443987</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="12"/>
+        <v>0.5329411584595718</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="12"/>
+        <v>0.8245546888754508</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="12"/>
+        <v>0.61598067958266678</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="5"/>
+        <v>0.5329411584595718</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="6"/>
-        <v>0.81598755877510232</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="4"/>
-        <v>0.68360949027161277</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34">
+        <v>0.5329411584595718</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="3"/>
+        <v>0.57026699999999997</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:I36" si="13">C9/$B36</f>
+        <v>1.0497135552293926</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="13"/>
+        <v>1.1348157968109676</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="13"/>
+        <v>1.3803656883529996</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="13"/>
+        <v>1.0712841528617296</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="13"/>
+        <v>0.87288410516477377</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="13"/>
+        <v>1.9972223537395641</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="13"/>
+        <v>1.5991877488965696</v>
+      </c>
+      <c r="J36">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="2"/>
-        <v>0.79624799999999996</v>
-      </c>
-      <c r="C34">
-        <f t="shared" ref="C34:I34" si="7">C7/$B34</f>
-        <v>1.2344809657292704</v>
-      </c>
-      <c r="D34">
+        <v>0.87288410516477377</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="6"/>
+        <v>0.87288410516477377</v>
+      </c>
+      <c r="M36">
         <f t="shared" si="7"/>
-        <v>5.2802016457184191</v>
-      </c>
-      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="3"/>
+        <v>1.9598100000000001</v>
+      </c>
+      <c r="C37">
+        <f t="shared" ref="C37:I37" si="14">C10/$B37</f>
+        <v>0.77724881493614173</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="14"/>
+        <v>0.4671422229705941</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="14"/>
+        <v>0.52029023221638837</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="14"/>
+        <v>0.97464039881417075</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="14"/>
+        <v>0.51033008301825178</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="14"/>
+        <v>0.85765967109056485</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="14"/>
+        <v>0.57924492680412898</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="5"/>
+        <v>0.51033008301825178</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="6"/>
+        <v>0.4671422229705941</v>
+      </c>
+      <c r="M37">
         <f t="shared" si="7"/>
-        <v>1.117418191317278</v>
-      </c>
-      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="3"/>
+        <v>0.65586800000000001</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ref="C38:I38" si="15">C11/$B38</f>
+        <v>0.98670159239359134</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="15"/>
+        <v>1.0102779827648247</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="15"/>
+        <v>1.0519662493062627</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="15"/>
+        <v>1.1313313044698019</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="15"/>
+        <v>0.77474278360889703</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="15"/>
+        <v>1.3375907957088926</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="15"/>
+        <v>1.1298767434910684</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="5"/>
+        <v>0.77474278360889703</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="6"/>
+        <v>0.77474278360889703</v>
+      </c>
+      <c r="M38">
         <f t="shared" si="7"/>
-        <v>0.83349031959891895</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="7"/>
-        <v>1.0258801277993792</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="7"/>
-        <v>1.3056233736222886</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="7"/>
-        <v>1.6220197727341232</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="4"/>
-        <v>1.0258801277993792</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="2"/>
-        <v>1.3063899999999999</v>
-      </c>
-      <c r="C35">
-        <f t="shared" ref="C35:I35" si="8">C8/$B35</f>
-        <v>0.89705218196710013</v>
-      </c>
-      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q38">
         <f t="shared" si="8"/>
-        <v>0.96674040676980078</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="8"/>
-        <v>0.66196005786939593</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="8"/>
-        <v>1.1933266482443987</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="8"/>
-        <v>0.5329411584595718</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="8"/>
-        <v>0.8245546888754508</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="8"/>
-        <v>0.61598067958266678</v>
-      </c>
-      <c r="J35">
-        <f t="shared" si="4"/>
-        <v>0.5329411584595718</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="2"/>
-        <v>0.57026699999999997</v>
-      </c>
-      <c r="C36">
-        <f t="shared" ref="C36:I36" si="9">C9/$B36</f>
-        <v>1.0497135552293926</v>
-      </c>
-      <c r="D36">
-        <f t="shared" si="9"/>
-        <v>1.1348157968109676</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="9"/>
-        <v>1.3803656883529996</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="9"/>
-        <v>1.0712841528617296</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="9"/>
-        <v>0.87288410516477377</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="9"/>
-        <v>1.9972223537395641</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="9"/>
-        <v>1.5991877488965696</v>
-      </c>
-      <c r="J36">
-        <f t="shared" si="4"/>
-        <v>0.87288410516477377</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="2"/>
-        <v>1.9598100000000001</v>
-      </c>
-      <c r="C37">
-        <f t="shared" ref="C37:I37" si="10">C10/$B37</f>
-        <v>0.77724881493614173</v>
-      </c>
-      <c r="D37">
-        <f t="shared" si="10"/>
-        <v>0.4671422229705941</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="10"/>
-        <v>0.52029023221638837</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="10"/>
-        <v>0.97464039881417075</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="10"/>
-        <v>0.51033008301825178</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="10"/>
-        <v>0.85765967109056485</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="10"/>
-        <v>0.57924492680412898</v>
-      </c>
-      <c r="J37">
-        <f t="shared" si="4"/>
-        <v>0.51033008301825178</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="2"/>
-        <v>0.65586800000000001</v>
-      </c>
-      <c r="C38">
-        <f t="shared" ref="C38:I38" si="11">C11/$B38</f>
-        <v>0.98670159239359134</v>
-      </c>
-      <c r="D38">
-        <f t="shared" si="11"/>
-        <v>1.0102779827648247</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="11"/>
-        <v>1.0519662493062627</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="11"/>
-        <v>1.1313313044698019</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="11"/>
-        <v>0.77474278360889703</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="11"/>
-        <v>1.3375907957088926</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="11"/>
-        <v>1.1298767434910684</v>
-      </c>
-      <c r="J38">
-        <f t="shared" si="4"/>
-        <v>0.77474278360889703</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>A38+1</f>
         <v>9</v>
       </c>
       <c r="B39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.03701</v>
       </c>
       <c r="C39">
-        <f t="shared" ref="C39:I39" si="12">C12/$B39</f>
+        <f t="shared" ref="C39:I39" si="16">C12/$B39</f>
         <v>0.77031040593811517</v>
       </c>
       <c r="D39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.4581469899509576</v>
       </c>
       <c r="E39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.782190563620208</v>
       </c>
       <c r="F39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.2742941860864698</v>
       </c>
       <c r="G39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.69277028586015788</v>
       </c>
       <c r="H39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1.3527179542564838</v>
       </c>
       <c r="I39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.73090461018846253</v>
       </c>
       <c r="J39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.69277028586015788</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L39">
+        <f t="shared" si="6"/>
+        <v>0.69277028586015788</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>A39+1</f>
         <v>10</v>
       </c>
       <c r="B40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.60263</v>
       </c>
       <c r="C40">
-        <f t="shared" ref="C40:I40" si="13">C13/$B40</f>
+        <f t="shared" ref="C40:I40" si="17">C13/$B40</f>
         <v>0.59851930888601856</v>
       </c>
       <c r="D40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2.2022300842989337</v>
       </c>
       <c r="E40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.55414537354224003</v>
       </c>
       <c r="F40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1.2532899047191179</v>
       </c>
       <c r="G40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.60595396317303429</v>
       </c>
       <c r="H40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1.025707742897612</v>
       </c>
       <c r="I40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.56789215227469847</v>
       </c>
       <c r="J40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.56789215227469847</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L40">
+        <f t="shared" si="6"/>
+        <v>0.55414537354224003</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="3"/>
+        <v>26.215199999999999</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ref="C41:I41" si="18">C14/$B41</f>
+        <v>0.97643733406573285</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="18"/>
+        <v>1.0035590039366473</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="18"/>
+        <v>0.93806265067594374</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="18"/>
+        <v>1.0907374347706675</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="18"/>
+        <v>0.96624858860508411</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="18"/>
+        <v>0.98296408190668005</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="18"/>
+        <v>0.95298529097622764</v>
+      </c>
+      <c r="J41">
         <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="2"/>
-        <v>26.215199999999999</v>
-      </c>
-      <c r="C41">
-        <f t="shared" ref="C41:I41" si="14">C14/$B41</f>
-        <v>0.97643733406573285</v>
-      </c>
-      <c r="D41">
-        <f t="shared" si="14"/>
-        <v>1.0035590039366473</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="14"/>
+        <v>0.95298529097622764</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="6"/>
         <v>0.93806265067594374</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="14"/>
-        <v>1.0907374347706675</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="14"/>
-        <v>0.96624858860508411</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="14"/>
-        <v>0.98296408190668005</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="14"/>
-        <v>0.95298529097622764</v>
-      </c>
-      <c r="J41">
-        <f t="shared" si="4"/>
-        <v>0.95298529097622764</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="3"/>
+        <v>24.2531</v>
+      </c>
+      <c r="C42">
+        <f t="shared" ref="C42:I42" si="19">C15/$B42</f>
+        <v>0.66404294708717648</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="19"/>
+        <v>0.62805991811356077</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="19"/>
+        <v>0.44462769707789934</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="19"/>
+        <v>0.59594443596901014</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="19"/>
+        <v>0.63959246446845974</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="19"/>
+        <v>0.77815619446586204</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="19"/>
+        <v>0.51165830347460739</v>
+      </c>
+      <c r="J42">
         <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="2"/>
-        <v>24.2531</v>
-      </c>
-      <c r="C42">
-        <f t="shared" ref="C42:I42" si="15">C15/$B42</f>
-        <v>0.66404294708717648</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="15"/>
-        <v>0.62805991811356077</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="15"/>
+        <v>0.51165830347460739</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="6"/>
         <v>0.44462769707789934</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="15"/>
-        <v>0.59594443596901014</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="15"/>
-        <v>0.63959246446845974</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="15"/>
-        <v>0.77815619446586204</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="15"/>
-        <v>0.51165830347460739</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="4"/>
-        <v>0.51165830347460739</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="3"/>
+        <v>77.0471</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C43:I43" si="20">C16/$B43</f>
+        <v>0.87080759691149956</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="20"/>
+        <v>0.87110741351718612</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="20"/>
+        <v>0.88817749143056646</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="20"/>
+        <v>0.94199392319762842</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="20"/>
+        <v>1.1265641406360525</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="20"/>
+        <v>1.0473294906622055</v>
+      </c>
+      <c r="J43">
         <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="2"/>
-        <v>77.0471</v>
-      </c>
-      <c r="C43">
-        <f t="shared" ref="C43:I43" si="16">C16/$B43</f>
+        <v>0.94199392319762842</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="6"/>
         <v>0.87080759691149956</v>
       </c>
-      <c r="E43">
-        <f t="shared" si="16"/>
-        <v>0.87110741351718612</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="16"/>
-        <v>0.88817749143056646</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="16"/>
-        <v>0.94199392319762842</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="16"/>
-        <v>1.1265641406360525</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="16"/>
-        <v>1.0473294906622055</v>
-      </c>
-      <c r="J43">
-        <f t="shared" si="4"/>
-        <v>0.94199392319762842</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="3"/>
+        <v>14.8528</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:I44" si="21">C17/$B44</f>
+        <v>0.91001696649789932</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="21"/>
+        <v>0.9736884627814284</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="21"/>
+        <v>0.64953678767639766</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="21"/>
+        <v>0.85787191640633409</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="21"/>
+        <v>0.80619815792308513</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="21"/>
+        <v>1.2760556932026283</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="21"/>
+        <v>0.63710815469137128</v>
+      </c>
+      <c r="J44">
         <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="B44">
-        <f t="shared" si="2"/>
-        <v>14.8528</v>
-      </c>
-      <c r="C44">
-        <f t="shared" ref="C44:I44" si="17">C17/$B44</f>
-        <v>0.91001696649789932</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="17"/>
-        <v>0.9736884627814284</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="17"/>
-        <v>0.64953678767639766</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="17"/>
-        <v>0.85787191640633409</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="17"/>
-        <v>0.80619815792308513</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="17"/>
-        <v>1.2760556932026283</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="17"/>
         <v>0.63710815469137128</v>
       </c>
-      <c r="J44">
-        <f t="shared" si="4"/>
+      <c r="L44">
+        <f t="shared" si="6"/>
         <v>0.63710815469137128</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="3"/>
+        <v>8.2829599999999992</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:I45" si="22">C18/$B45</f>
+        <v>0.98421578759284123</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="22"/>
+        <v>1.0890285598385119</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="22"/>
+        <v>0.85162067666631258</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="22"/>
+        <v>0.97817205443464661</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="22"/>
+        <v>1.0181179191979681</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="22"/>
+        <v>1.0844178892569807</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="22"/>
+        <v>0.86348600017385091</v>
+      </c>
+      <c r="J45">
         <f t="shared" si="5"/>
+        <v>0.86348600017385091</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="6"/>
+        <v>0.85162067666631258</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="3"/>
+        <v>32.504100000000001</v>
+      </c>
+      <c r="C46">
+        <f t="shared" ref="C46:I46" si="23">C19/$B46</f>
+        <v>1.1306665928298276</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="23"/>
+        <v>0.99922471319002837</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="23"/>
+        <v>0.898754310994613</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="23"/>
+        <v>0.99754492510175641</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="23"/>
+        <v>1.0708710593432826</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="23"/>
+        <v>1.6112244301488119</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="23"/>
+        <v>0.84194916948938747</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="5"/>
+        <v>0.84194916948938747</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="6"/>
+        <v>0.84194916948938747</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="9"/>
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="3"/>
+        <v>0.45866099999999999</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:I47" si="24">C20/$B47</f>
+        <v>1.5434035158864607</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="24"/>
+        <v>1.181870706251458</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="24"/>
+        <v>1.0903979191603386</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="24"/>
+        <v>1.0078445736611572</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="24"/>
+        <v>1.3177161345743369</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="24"/>
+        <v>1.1645136604158626</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="24"/>
+        <v>1.0659877338600841</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="5"/>
+        <v>1.0659877338600841</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="6"/>
+        <v>1.0078445736611572</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="9"/>
+        <v>18</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="3"/>
+        <v>1.0772200000000001</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:I48" si="25">C21/$B48</f>
+        <v>0.55141568110506667</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="25"/>
+        <v>3.1945749243422883</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="25"/>
+        <v>0.497166781158909</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="25"/>
+        <v>1.0478546629286496</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="25"/>
+        <v>0.49025640073522581</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="25"/>
+        <v>0.91462839531386342</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="25"/>
+        <v>0.63725330016152681</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="5"/>
+        <v>0.49025640073522581</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="6"/>
+        <v>0.49025640073522581</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="3"/>
+        <v>2.0551599999999999</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49:I49" si="26">C22/$B49</f>
+        <v>1.1629897428910645</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="26"/>
+        <v>2.6264329784542322</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="26"/>
+        <v>1.3303051830514412</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="26"/>
+        <v>1.1598221063080247</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="26"/>
+        <v>0.75755658926798886</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="26"/>
+        <v>1.9840985616691644</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="26"/>
+        <v>0.90381770762373748</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="5"/>
+        <v>0.75755658926798886</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="6"/>
+        <v>0.75755658926798886</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="9"/>
+        <v>20</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="3"/>
+        <v>2.3985599999999998</v>
+      </c>
+      <c r="C50">
+        <f t="shared" ref="C50:I50" si="27">C23/$B50</f>
+        <v>1.0372348409045429</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="27"/>
+        <v>1.6369655126409179</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="27"/>
+        <v>0.80053031819091458</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="27"/>
+        <v>0.94816473217263708</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="27"/>
+        <v>2.3599159495697419</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="27"/>
+        <v>2.3544668467747316</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="27"/>
+        <v>1.4828647188312989</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="5"/>
+        <v>1.4828647188312989</v>
+      </c>
+      <c r="L50">
+        <f t="shared" si="6"/>
+        <v>0.80053031819091458</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="9"/>
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="3"/>
+        <v>2.2712699999999999</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:I51" si="28">C24/$B51</f>
+        <v>0.44802247200905221</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="28"/>
+        <v>0.72074654268316851</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="28"/>
+        <v>0.90855776724035453</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="28"/>
+        <v>0.92708484680377057</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="28"/>
+        <v>0.50225204401061962</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="28"/>
+        <v>37.023383393431871</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="28"/>
+        <v>244.12245131578368</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="5"/>
+        <v>0.50225204401061962</v>
+      </c>
+      <c r="L51">
+        <f t="shared" si="6"/>
+        <v>0.44802247200905221</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="9"/>
+        <v>22</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="3"/>
+        <v>3.2597499999999999</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ref="C52:I52" si="29">C25/$B52</f>
+        <v>0.74217347956131596</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="29"/>
+        <v>1.1110882736406167</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="29"/>
+        <v>0.8939611933430478</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="29"/>
+        <v>1.4192836873993404</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="29"/>
+        <v>0.64787483702737936</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="29"/>
+        <v>17.145026459084285</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="29"/>
+        <v>0.61169108060434085</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="5"/>
+        <v>0.61169108060434085</v>
+      </c>
+      <c r="L52">
+        <f t="shared" si="6"/>
+        <v>0.61169108060434085</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="9"/>
+        <v>23</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="3"/>
+        <v>28.321100000000001</v>
+      </c>
+      <c r="C53">
+        <f t="shared" ref="C53:I53" si="30">C26/$B53</f>
+        <v>0.13892680722147091</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="30"/>
+        <v>1.457973030708553</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="30"/>
+        <v>0.2559625155802564</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="30"/>
+        <v>0.88681583695548549</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="30"/>
+        <v>0.11517878895946837</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="30"/>
+        <v>0.12993563103128056</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="30"/>
+        <v>0.12642552725706274</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="5"/>
+        <v>0.11517878895946837</v>
+      </c>
+      <c r="L53">
+        <f t="shared" si="6"/>
+        <v>0.11517878895946837</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>15</v>
       </c>
-      <c r="B45">
-        <f t="shared" si="2"/>
-        <v>8.2829599999999992</v>
-      </c>
-      <c r="C45">
-        <f t="shared" ref="C45:I45" si="18">C18/$B45</f>
-        <v>0.98421578759284123</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="18"/>
-        <v>1.0890285598385119</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="18"/>
-        <v>0.85162067666631258</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="18"/>
-        <v>0.97817205443464661</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="18"/>
-        <v>1.0181179191979681</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="18"/>
-        <v>1.0844178892569807</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="18"/>
-        <v>0.86348600017385091</v>
-      </c>
-      <c r="J45">
-        <f t="shared" si="4"/>
-        <v>0.86348600017385091</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="B46">
-        <f t="shared" si="2"/>
-        <v>32.504100000000001</v>
-      </c>
-      <c r="C46">
-        <f t="shared" ref="C46:I46" si="19">C19/$B46</f>
-        <v>1.1306665928298276</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="19"/>
-        <v>0.99922471319002837</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="19"/>
-        <v>0.898754310994613</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="19"/>
-        <v>0.99754492510175641</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="19"/>
-        <v>1.0708710593432826</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="19"/>
-        <v>1.6112244301488119</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="19"/>
-        <v>0.84194916948938747</v>
-      </c>
-      <c r="J46">
-        <f t="shared" si="4"/>
-        <v>0.84194916948938747</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <f t="shared" si="5"/>
+      <c r="B54">
+        <f>ROUND(AVERAGE(B31:B53)*1000,2)</f>
+        <v>10151.540000000001</v>
+      </c>
+      <c r="C54">
+        <f t="shared" ref="C54:J54" si="31">ROUND(AVERAGE(C31:C53)*1000,2)</f>
+        <v>874.18</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="31"/>
+        <v>1447.42</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="31"/>
+        <v>818.41</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="31"/>
+        <v>1011.59</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="31"/>
+        <v>822.8</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="31"/>
+        <v>3458.15</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="31"/>
+        <v>11468.95</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="31"/>
+        <v>740.33</v>
+      </c>
+      <c r="L54" t="s">
         <v>17</v>
       </c>
-      <c r="B47">
-        <f t="shared" si="2"/>
-        <v>0.45866099999999999</v>
-      </c>
-      <c r="C47">
-        <f t="shared" ref="C47:I47" si="20">C20/$B47</f>
-        <v>1.5434035158864607</v>
-      </c>
-      <c r="D47">
-        <f t="shared" si="20"/>
-        <v>1.181870706251458</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="20"/>
-        <v>1.0903979191603386</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="20"/>
-        <v>1.0078445736611572</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="20"/>
-        <v>1.3177161345743369</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="20"/>
-        <v>1.1645136604158626</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="20"/>
-        <v>1.0659877338600841</v>
-      </c>
-      <c r="J47">
-        <f t="shared" si="4"/>
-        <v>1.0659877338600841</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="2"/>
-        <v>1.0772200000000001</v>
-      </c>
-      <c r="C48">
-        <f t="shared" ref="C48:I48" si="21">C21/$B48</f>
-        <v>0.55141568110506667</v>
-      </c>
-      <c r="D48">
-        <f t="shared" si="21"/>
-        <v>3.1945749243422883</v>
-      </c>
-      <c r="E48">
-        <f t="shared" si="21"/>
-        <v>0.497166781158909</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="21"/>
-        <v>1.0478546629286496</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="21"/>
-        <v>0.49025640073522581</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="21"/>
-        <v>0.91462839531386342</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="21"/>
-        <v>0.63725330016152681</v>
-      </c>
-      <c r="J48">
-        <f t="shared" si="4"/>
-        <v>0.49025640073522581</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="B49">
-        <f t="shared" si="2"/>
-        <v>2.0551599999999999</v>
-      </c>
-      <c r="C49">
-        <f t="shared" ref="C49:I49" si="22">C22/$B49</f>
-        <v>1.1629897428910645</v>
-      </c>
-      <c r="D49">
-        <f t="shared" si="22"/>
-        <v>2.6264329784542322</v>
-      </c>
-      <c r="E49">
-        <f t="shared" si="22"/>
-        <v>1.3303051830514412</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="22"/>
-        <v>1.1598221063080247</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="22"/>
-        <v>0.75755658926798886</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="22"/>
-        <v>1.9840985616691644</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="22"/>
-        <v>0.90381770762373748</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="4"/>
-        <v>0.75755658926798886</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="B50">
-        <f t="shared" si="2"/>
-        <v>2.3985599999999998</v>
-      </c>
-      <c r="C50">
-        <f t="shared" ref="C50:I50" si="23">C23/$B50</f>
-        <v>1.0372348409045429</v>
-      </c>
-      <c r="D50">
-        <f t="shared" si="23"/>
-        <v>1.6369655126409179</v>
-      </c>
-      <c r="E50">
-        <f t="shared" si="23"/>
-        <v>0.80053031819091458</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="23"/>
-        <v>0.94816473217263708</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="23"/>
-        <v>2.3599159495697419</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="23"/>
-        <v>2.3544668467747316</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="23"/>
-        <v>1.4828647188312989</v>
-      </c>
-      <c r="J50">
-        <f t="shared" si="4"/>
-        <v>1.4828647188312989</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="B51">
-        <f t="shared" si="2"/>
-        <v>2.2712699999999999</v>
-      </c>
-      <c r="C51">
-        <f t="shared" ref="C51:I51" si="24">C24/$B51</f>
-        <v>0.44802247200905221</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="24"/>
-        <v>0.72074654268316851</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="24"/>
-        <v>0.90855776724035453</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="24"/>
-        <v>0.92708484680377057</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="24"/>
-        <v>0.50225204401061962</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="24"/>
-        <v>37.023383393431871</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="24"/>
-        <v>244.12245131578368</v>
-      </c>
-      <c r="J51">
-        <f t="shared" si="4"/>
-        <v>0.50225204401061962</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="B52">
-        <f t="shared" si="2"/>
-        <v>3.2597499999999999</v>
-      </c>
-      <c r="C52">
-        <f t="shared" ref="C52:I52" si="25">C25/$B52</f>
-        <v>0.74217347956131596</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="25"/>
-        <v>1.1110882736406167</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="25"/>
-        <v>0.8939611933430478</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="25"/>
-        <v>1.4192836873993404</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="25"/>
-        <v>0.64787483702737936</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="25"/>
-        <v>17.145026459084285</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="25"/>
-        <v>0.61169108060434085</v>
-      </c>
-      <c r="J52">
-        <f t="shared" si="4"/>
-        <v>0.61169108060434085</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="2"/>
-        <v>28.321100000000001</v>
-      </c>
-      <c r="C53">
-        <f t="shared" ref="C53:I53" si="26">C26/$B53</f>
-        <v>0.13892680722147091</v>
-      </c>
-      <c r="D53">
-        <f t="shared" si="26"/>
-        <v>1.457973030708553</v>
-      </c>
-      <c r="E53">
-        <f t="shared" si="26"/>
-        <v>0.2559625155802564</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="26"/>
-        <v>0.88681583695548549</v>
-      </c>
-      <c r="G53">
-        <f t="shared" si="26"/>
-        <v>0.11517878895946837</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="26"/>
-        <v>0.12993563103128056</v>
-      </c>
-      <c r="I53">
-        <f t="shared" si="26"/>
-        <v>0.12642552725706274</v>
-      </c>
-      <c r="J53">
-        <f t="shared" si="4"/>
-        <v>0.11517878895946837</v>
+      <c r="M54">
+        <f>AVERAGE(M31:M53)*100</f>
+        <v>8.695652173913043</v>
+      </c>
+      <c r="N54">
+        <f t="shared" ref="N54:R54" si="32">AVERAGE(N31:N53)*100</f>
+        <v>4.3478260869565215</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="32"/>
+        <v>26.086956521739129</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="32"/>
+        <v>8.695652173913043</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="32"/>
+        <v>52.173913043478258</v>
+      </c>
+      <c r="R54">
+        <f>SUM(M54:Q54)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>